<commit_message>
Increase the amount of ambient heat available in SRV in 2018-2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_Historic_Bounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SuppXLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{297978D7-01DC-4339-A28F-284DCB5B44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B43B1A8C-CA03-4E23-91D8-C950F79D4750}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF6620F-668C-4196-AF49-F302756BBD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="20" r:id="rId1"/>
@@ -5708,7 +5708,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>30480</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -6028,17 +6028,17 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="10" width="8.109375" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -8882,14 +8882,14 @@
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -9379,7 +9379,7 @@
       </c>
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="2:10" ht="15" thickBot="1">
+    <row r="42" spans="2:10" ht="15.75" thickBot="1">
       <c r="B42" s="29" t="s">
         <v>227</v>
       </c>
@@ -9605,19 +9605,19 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X60" sqref="X60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="32" width="6.88671875" customWidth="1"/>
-    <col min="33" max="33" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="32" width="6.85546875" customWidth="1"/>
+    <col min="33" max="33" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="21">
@@ -9642,7 +9642,7 @@
       <c r="M5" s="37"/>
       <c r="N5" s="37"/>
     </row>
-    <row r="6" spans="1:34" ht="15" thickBot="1">
+    <row r="6" spans="1:34" ht="15.75" thickBot="1">
       <c r="B6" s="36" t="s">
         <v>228</v>
       </c>
@@ -11311,7 +11311,7 @@
       <c r="M25" s="37"/>
       <c r="N25" s="37"/>
     </row>
-    <row r="26" spans="1:34" ht="15" thickBot="1">
+    <row r="26" spans="1:34" ht="15.75" thickBot="1">
       <c r="B26" s="36" t="s">
         <v>228</v>
       </c>
@@ -12979,7 +12979,7 @@
       <c r="M47" s="37"/>
       <c r="N47" s="37"/>
     </row>
-    <row r="48" spans="1:34" ht="15" thickBot="1">
+    <row r="48" spans="1:34" ht="15.75" thickBot="1">
       <c r="B48" s="36" t="s">
         <v>228</v>
       </c>
@@ -14631,11 +14631,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14746,17 +14746,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -14907,18 +14907,18 @@
       <selection activeCell="B2" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -15070,10 +15070,10 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="7" width="12" customWidth="1"/>
   </cols>
@@ -15083,17 +15083,17 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="57" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="57" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="56" t="s">
         <v>393</v>
       </c>
@@ -15219,12 +15219,12 @@
         <v>117109</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="57" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6">
+    <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="56" t="s">
         <v>393</v>
       </c>
@@ -15360,12 +15360,12 @@
         <v>25336</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.6">
+    <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="57" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.6">
+    <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="56" t="s">
         <v>393</v>
       </c>
@@ -15443,7 +15443,7 @@
         <v>2659</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="15.6">
+    <row r="40" spans="1:29" ht="15.75">
       <c r="B40" s="55" t="s">
         <v>386</v>
       </c>
@@ -15742,7 +15742,7 @@
       </c>
       <c r="C49" s="402"/>
     </row>
-    <row r="50" spans="2:3" ht="15" thickBot="1">
+    <row r="50" spans="2:3" ht="15.75" thickBot="1">
       <c r="B50" s="46" t="s">
         <v>381</v>
       </c>
@@ -15750,7 +15750,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15" thickBot="1">
+    <row r="51" spans="2:3" ht="15.75" thickBot="1">
       <c r="B51" s="45" t="s">
         <v>379</v>
       </c>
@@ -16381,7 +16381,7 @@
       <c r="C131" s="389"/>
       <c r="D131" s="389"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6">
+    <row r="132" spans="1:9" ht="15.75">
       <c r="A132" s="390" t="s">
         <v>536</v>
       </c>
@@ -16389,7 +16389,7 @@
       <c r="C132" s="389"/>
       <c r="D132" s="389"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6">
+    <row r="134" spans="1:9" ht="15.75">
       <c r="A134" s="390" t="s">
         <v>401</v>
       </c>
@@ -16405,7 +16405,7 @@
       <c r="C135" s="389"/>
       <c r="D135" s="389"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6">
+    <row r="137" spans="1:9" ht="15.75">
       <c r="A137" s="387" t="s">
         <v>393</v>
       </c>
@@ -16657,7 +16657,7 @@
       <c r="F149" s="389"/>
       <c r="G149" s="389"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6">
+    <row r="150" spans="1:9" ht="15.75">
       <c r="A150" s="390" t="s">
         <v>536</v>
       </c>
@@ -16668,7 +16668,7 @@
       <c r="F150" s="389"/>
       <c r="G150" s="389"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6">
+    <row r="152" spans="1:9" ht="15.75">
       <c r="A152" s="390" t="s">
         <v>400</v>
       </c>
@@ -16690,7 +16690,7 @@
       <c r="F153" s="389"/>
       <c r="G153" s="389"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6">
+    <row r="155" spans="1:9" ht="15.75">
       <c r="A155" s="390" t="s">
         <v>393</v>
       </c>
@@ -16919,7 +16919,7 @@
       <c r="F166" s="389"/>
       <c r="G166" s="389"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6">
+    <row r="167" spans="1:9" ht="15.75">
       <c r="A167" s="390" t="s">
         <v>536</v>
       </c>
@@ -16930,7 +16930,7 @@
       <c r="F167" s="389"/>
       <c r="G167" s="389"/>
     </row>
-    <row r="169" spans="1:9" ht="15.6">
+    <row r="169" spans="1:9" ht="15.75">
       <c r="A169" s="390" t="s">
         <v>394</v>
       </c>
@@ -16952,7 +16952,7 @@
       <c r="F170" s="389"/>
       <c r="G170" s="389"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6">
+    <row r="172" spans="1:9" ht="15.75">
       <c r="A172" s="390" t="s">
         <v>393</v>
       </c>
@@ -17164,46 +17164,46 @@
       <selection pane="bottomRight" activeCell="AS53" sqref="AS53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="12"/>
-    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="5.5546875" style="7" customWidth="1"/>
-    <col min="31" max="31" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.6640625" style="7" customWidth="1"/>
-    <col min="33" max="33" width="5.5546875" style="7" customWidth="1"/>
-    <col min="34" max="34" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="5.5703125" style="7" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.7109375" style="7" customWidth="1"/>
+    <col min="33" max="33" width="5.5703125" style="7" customWidth="1"/>
+    <col min="34" max="34" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.109375" style="7"/>
-    <col min="45" max="45" width="9.109375" style="9"/>
-    <col min="46" max="16384" width="9.109375" style="7"/>
+    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="7"/>
+    <col min="45" max="45" width="9.140625" style="9"/>
+    <col min="46" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="105.75" customHeight="1" thickBot="1">
@@ -24448,45 +24448,45 @@
       <selection pane="bottomRight" activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
     <col min="7" max="7" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
-    <col min="27" max="27" width="7.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
+    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="35" width="7" style="7" customWidth="1"/>
-    <col min="36" max="36" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.5546875" style="7" customWidth="1"/>
-    <col min="39" max="39" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.5546875" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.109375" style="7"/>
+    <col min="36" max="36" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.5703125" style="7" customWidth="1"/>
+    <col min="39" max="39" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.5703125" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="105.75" customHeight="1" thickBot="1">
@@ -31711,41 +31711,41 @@
       <selection pane="bottomRight" activeCell="AQ45" sqref="AQ45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="12"/>
-    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.109375" style="7"/>
+    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
@@ -38738,7 +38738,7 @@
       <c r="AP76" s="23"/>
       <c r="AQ76" s="23"/>
     </row>
-    <row r="77" spans="1:43" ht="14.4">
+    <row r="77" spans="1:43" ht="15">
       <c r="A77" s="363" t="s">
         <v>437</v>
       </c>
@@ -38785,7 +38785,7 @@
       <c r="AP77" s="23"/>
       <c r="AQ77" s="23"/>
     </row>
-    <row r="78" spans="1:43" ht="14.4">
+    <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
         <v>438</v>
       </c>
@@ -38832,7 +38832,7 @@
       <c r="AP78" s="23"/>
       <c r="AQ78" s="23"/>
     </row>
-    <row r="79" spans="1:43" ht="14.4">
+    <row r="79" spans="1:43" ht="15">
       <c r="A79" s="364" t="s">
         <v>153</v>
       </c>
@@ -38879,7 +38879,7 @@
       <c r="AP79" s="369"/>
       <c r="AQ79" s="366"/>
     </row>
-    <row r="80" spans="1:43" ht="14.4">
+    <row r="80" spans="1:43" ht="15">
       <c r="A80" s="364" t="s">
         <v>154</v>
       </c>
@@ -39033,41 +39033,41 @@
       <selection pane="bottomRight" activeCell="AA65" sqref="AA65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="38.109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="12"/>
-    <col min="6" max="6" width="6.109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="6.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.44140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="5.44140625" style="14" customWidth="1"/>
-    <col min="27" max="27" width="8.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="5.5546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" style="14" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5703125" style="7" customWidth="1"/>
     <col min="34" max="34" width="6" style="7" customWidth="1"/>
     <col min="35" max="36" width="7" style="7" customWidth="1"/>
-    <col min="37" max="40" width="5.5546875" style="7" customWidth="1"/>
-    <col min="41" max="41" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.109375" style="7"/>
+    <col min="37" max="40" width="5.5703125" style="7" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="105.75" customHeight="1" thickBot="1">
@@ -46060,7 +46060,7 @@
       <c r="AP76" s="23"/>
       <c r="AQ76" s="23"/>
     </row>
-    <row r="77" spans="1:43" ht="14.4">
+    <row r="77" spans="1:43" ht="15">
       <c r="A77" s="363" t="s">
         <v>443</v>
       </c>
@@ -46107,7 +46107,7 @@
       <c r="AP77" s="23"/>
       <c r="AQ77" s="23"/>
     </row>
-    <row r="78" spans="1:43" ht="14.4">
+    <row r="78" spans="1:43" ht="15">
       <c r="A78" s="24" t="s">
         <v>444</v>
       </c>
@@ -46154,7 +46154,7 @@
       <c r="AP78" s="23"/>
       <c r="AQ78" s="23"/>
     </row>
-    <row r="79" spans="1:43" ht="14.4">
+    <row r="79" spans="1:43" ht="15">
       <c r="A79" s="364" t="s">
         <v>153</v>
       </c>
@@ -46201,7 +46201,7 @@
       <c r="AP79" s="369"/>
       <c r="AQ79" s="366"/>
     </row>
-    <row r="80" spans="1:43" ht="14.4">
+    <row r="80" spans="1:43" ht="15">
       <c r="A80" s="364" t="s">
         <v>154</v>
       </c>
@@ -46352,35 +46352,35 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:30">
@@ -46851,7 +46851,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -47093,7 +47093,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>30480</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -47119,9 +47119,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="21"/>
+    <col min="1" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -47153,18 +47153,18 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -47542,11 +47542,11 @@
       <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
@@ -47555,7 +47555,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:11" ht="15" thickBot="1">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -47977,15 +47977,15 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -48004,7 +48004,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1">
       <c r="B6" s="29" t="s">
         <v>461</v>
       </c>
@@ -48242,12 +48242,12 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48256,7 +48256,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48329,12 +48329,12 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48343,7 +48343,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48416,12 +48416,12 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48430,7 +48430,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48819,16 +48819,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -48837,7 +48837,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
         <v>227</v>
       </c>
@@ -48877,21 +48877,21 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:$D$3)</f>
         <v>IE,National</v>
       </c>
-      <c r="F4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AM$57),1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="G4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AM$57),1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="H4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AM$57),1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="I4" s="19">
-        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AM$57),1)</f>
-        <v>0.7</v>
+      <c r="F4" s="375">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2018'!$AM$57),1)*2</f>
+        <v>1.4</v>
+      </c>
+      <c r="G4" s="375">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2019'!$AM$57),1)*2</f>
+        <v>1.4</v>
+      </c>
+      <c r="H4" s="375">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2020'!$AM$57),1)*2</f>
+        <v>1.4</v>
+      </c>
+      <c r="I4" s="375">
+        <f>ROUNDUP(Conversions!$B$2*SUM('EB2021'!$AM$57),1)*2</f>
+        <v>1.4</v>
       </c>
       <c r="J4">
         <v>1</v>

</xml_diff>